<commit_message>
up to Emerson 9/23
</commit_message>
<xml_diff>
--- a/rcp.xlsx
+++ b/rcp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="615" windowWidth="27555" windowHeight="11805"/>
+    <workbookView xWindow="720" yWindow="675" windowWidth="27555" windowHeight="11745"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3542" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3617" uniqueCount="47">
   <si>
     <t>Economist/YouGov</t>
   </si>
@@ -736,13 +736,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO138"/>
+  <dimension ref="A1:AO141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AS120" sqref="AS120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.42578125" style="5" bestFit="1" customWidth="1"/>
@@ -750,31 +750,31 @@
     <col min="4" max="4" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="1.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="1.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="1.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="1.42578125" style="5" bestFit="1" customWidth="1"/>
@@ -784,7 +784,7 @@
     <col min="38" max="38" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="1.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="24.140625" style="5"/>
+    <col min="41" max="16384" width="8.5703125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="24" x14ac:dyDescent="0.25">
@@ -4344,7 +4344,7 @@
       <c r="F30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="9">
         <v>28</v>
       </c>
       <c r="H30" s="31" t="s">
@@ -17621,6 +17621,372 @@
         <v>19</v>
       </c>
       <c r="AN138" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A139" s="5">
+        <v>11</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C139" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E139" s="7">
+        <v>43724</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G139" s="9">
+        <v>32</v>
+      </c>
+      <c r="H139" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I139" s="9">
+        <v>19</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K139" s="5">
+        <v>20</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M139" s="9">
+        <v>6</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O139" s="9">
+        <v>5</v>
+      </c>
+      <c r="P139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q139" s="5">
+        <v>3</v>
+      </c>
+      <c r="R139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S139" s="5">
+        <v>3</v>
+      </c>
+      <c r="T139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U139" s="5">
+        <v>3</v>
+      </c>
+      <c r="V139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W139" s="5">
+        <v>1</v>
+      </c>
+      <c r="X139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y139" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA139" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC139" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD139" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE139" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF139" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG139" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH139" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI139" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ139" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK139" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL139" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM139" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN139" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A140" s="5">
+        <v>15</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C140" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E140" s="7">
+        <v>43728</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G140" s="9">
+        <v>31</v>
+      </c>
+      <c r="H140" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I140" s="9">
+        <v>16</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K140" s="5">
+        <v>14</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M140" s="9">
+        <v>5</v>
+      </c>
+      <c r="N140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O140" s="9">
+        <v>5</v>
+      </c>
+      <c r="P140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q140" s="5">
+        <v>2</v>
+      </c>
+      <c r="R140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S140" s="5">
+        <v>2</v>
+      </c>
+      <c r="T140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U140" s="5">
+        <v>4</v>
+      </c>
+      <c r="V140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W140" s="5">
+        <v>1</v>
+      </c>
+      <c r="X140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y140" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA140" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC140" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD140" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE140" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF140" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG140" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH140" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI140" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ140" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK140" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL140" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM140" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN140" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A141" s="5">
+        <v>4</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C141" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E141" s="7">
+        <v>43729</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G141" s="9">
+        <v>25</v>
+      </c>
+      <c r="H141" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I141" s="9">
+        <v>22</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K141" s="5">
+        <v>23</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M141" s="9">
+        <v>4</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O141" s="9">
+        <v>6</v>
+      </c>
+      <c r="P141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q141" s="5">
+        <v>8</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S141" s="5">
+        <v>2</v>
+      </c>
+      <c r="T141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U141" s="5">
+        <v>1</v>
+      </c>
+      <c r="V141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W141" s="5">
+        <v>1</v>
+      </c>
+      <c r="X141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y141" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA141" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC141" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD141" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE141" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF141" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG141" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH141" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI141" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ141" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK141" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL141" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM141" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN141" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>